<commit_message>
Improved the loading file logic, and added protection to the code in case a ptr does not exist and in case any view method is called twice
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Homer\Documents\Programmation_project\SourcesPersonal\GraphViewerGUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE80A3C3-E99F-41FF-8A17-FD02E330C8B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB9B31B-4F83-4192-9FA7-0C30B666A5A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7035" yWindow="1440" windowWidth="17190" windowHeight="11835" xr2:uid="{8304BE1A-A5AF-42C4-9AC3-9E9523FB1C29}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Node</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>is automatically constructed with everything needed</t>
-  </si>
-  <si>
-    <t>isLeaf (1 or 0)</t>
   </si>
 </sst>
 </file>
@@ -451,7 +448,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,9 +483,6 @@
       <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">

</xml_diff>